<commit_message>
Kill One Bird with Two Stones
I missed the first time
</commit_message>
<xml_diff>
--- a/Cruise.xlsx
+++ b/Cruise.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enver\Documents\GitHub\SpringBreak\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>M</t>
   </si>
@@ -193,6 +198,9 @@
   </si>
   <si>
     <t>Victory</t>
+  </si>
+  <si>
+    <t>Kate Upton</t>
   </si>
 </sst>
 </file>
@@ -331,6 +339,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -378,7 +389,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,7 +424,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -739,7 +750,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,6 +1040,9 @@
       <c r="F11" t="s">
         <v>56</v>
       </c>
+      <c r="H11" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>